<commit_message>
fix mapping for new categories
</commit_message>
<xml_diff>
--- a/static/data/dataset.xlsx
+++ b/static/data/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valizanadya/Documents/KULIAH/term 3/PBP/nyarap-at-depok/nyarap-at-depok/static/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valizanadya/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358ACFA8-8948-AB4D-BB83-19C9065C6CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CDF815C-B153-5A43-98D3-A17018ECBB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="730">
   <si>
     <t>Kategori</t>
   </si>
@@ -1725,9 +1725,6 @@
     <t>https://satekhas.sarirasa.co.id/admin/uploads/news-promotion/articles/Menu_Spesial_Imlek_Sate_Khas_Senayan.jpg</t>
   </si>
   <si>
-    <t>Makanan Sehat</t>
-  </si>
-  <si>
     <t>Jl. Komjen.Pol.M.Jasin No.9, Tugu, Kec. Cimanggis, Kota Depok, Jawa Barat 16451</t>
   </si>
   <si>
@@ -1771,9 +1768,6 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/p/AF1QipNVgJSqVOKnylcJMgYz3k4TkjnoPdC429Q5788_=s1360-w1360-h1020</t>
-  </si>
-  <si>
-    <t>Makanan Berat</t>
   </si>
   <si>
     <t>https://i.gojekapi.com/darkroom/gofood-indonesia/v2/images/uploads/cc291c88-617c-4820-953e-3911aad9286b_IMG_20200915_101741_459.jpg</t>
@@ -2314,6 +2308,15 @@
       </rPr>
       <t>g</t>
     </r>
+  </si>
+  <si>
+    <t>https://univindonesia-my.sharepoint.com/personal/valiza_nadya_office_ui_ac_id/Documents/dataset.xlsx?web=1</t>
+  </si>
+  <si>
+    <t>Sarapan Berat</t>
+  </si>
+  <si>
+    <t>Sarapan Sehat</t>
   </si>
 </sst>
 </file>
@@ -2518,7 +2521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2582,6 +2585,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3717,8 +3721,8 @@
   </sheetPr>
   <dimension ref="A1:L214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J130" sqref="J130"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4276,7 +4280,7 @@
         <v>10000</v>
       </c>
       <c r="J16" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -5162,8 +5166,8 @@
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" ht="14.75" customHeight="1">
-      <c r="A43" t="s">
-        <v>566</v>
+      <c r="A43" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B43" t="s">
         <v>186</v>
@@ -5181,7 +5185,7 @@
         <v>189</v>
       </c>
       <c r="G43" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H43" t="s">
         <v>57</v>
@@ -5190,14 +5194,14 @@
         <v>6000</v>
       </c>
       <c r="J43" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A44" t="s">
-        <v>566</v>
+      <c r="A44" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B44" t="s">
         <v>186</v>
@@ -5215,7 +5219,7 @@
         <v>192</v>
       </c>
       <c r="G44" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H44" t="s">
         <v>17</v>
@@ -5224,14 +5228,14 @@
         <v>13000</v>
       </c>
       <c r="J44" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A45" t="s">
-        <v>566</v>
+      <c r="A45" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B45" t="s">
         <v>195</v>
@@ -5246,10 +5250,10 @@
         <v>97</v>
       </c>
       <c r="F45" t="s">
+        <v>570</v>
+      </c>
+      <c r="G45" s="36" t="s">
         <v>571</v>
-      </c>
-      <c r="G45" s="36" t="s">
-        <v>572</v>
       </c>
       <c r="H45" t="s">
         <v>17</v>
@@ -5258,14 +5262,14 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A46" t="s">
-        <v>566</v>
+      <c r="A46" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B46" t="s">
         <v>195</v>
@@ -5283,7 +5287,7 @@
         <v>35</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
@@ -5292,14 +5296,14 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A47" t="s">
-        <v>566</v>
+      <c r="A47" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B47" t="s">
         <v>195</v>
@@ -5317,7 +5321,7 @@
         <v>198</v>
       </c>
       <c r="G47" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H47" t="s">
         <v>30</v>
@@ -5326,14 +5330,14 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A48" t="s">
-        <v>566</v>
+      <c r="A48" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B48" t="s">
         <v>200</v>
@@ -5360,14 +5364,14 @@
         <v>0</v>
       </c>
       <c r="J48" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A49" t="s">
-        <v>566</v>
+      <c r="A49" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B49" t="s">
         <v>200</v>
@@ -5394,14 +5398,14 @@
         <v>0</v>
       </c>
       <c r="J49" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A50" t="s">
-        <v>566</v>
+      <c r="A50" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B50" t="s">
         <v>208</v>
@@ -5428,14 +5432,14 @@
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A51" t="s">
-        <v>566</v>
+      <c r="A51" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B51" t="s">
         <v>208</v>
@@ -5462,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
@@ -5485,7 +5489,7 @@
         <v>15</v>
       </c>
       <c r="G52" s="36" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H52" t="s">
         <v>17</v>
@@ -5494,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
@@ -5514,10 +5518,10 @@
       </c>
       <c r="E53"/>
       <c r="F53" t="s">
+        <v>578</v>
+      </c>
+      <c r="G53" s="36" t="s">
         <v>579</v>
-      </c>
-      <c r="G53" s="36" t="s">
-        <v>580</v>
       </c>
       <c r="H53" t="s">
         <v>17</v>
@@ -5526,14 +5530,14 @@
         <v>2500</v>
       </c>
       <c r="J53" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A54" t="s">
-        <v>582</v>
+      <c r="A54" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B54" t="s">
         <v>219</v>
@@ -5560,14 +5564,14 @@
         <v>20000</v>
       </c>
       <c r="J54" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A55" t="s">
-        <v>582</v>
+      <c r="A55" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B55" t="s">
         <v>219</v>
@@ -5594,14 +5598,14 @@
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A56" t="s">
-        <v>582</v>
+      <c r="A56" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B56" t="s">
         <v>225</v>
@@ -5628,14 +5632,14 @@
         <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1">
-      <c r="A57" t="s">
-        <v>582</v>
+      <c r="A57" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B57" t="s">
         <v>225</v>
@@ -5662,14 +5666,14 @@
         <v>13000</v>
       </c>
       <c r="J57" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A58" t="s">
-        <v>582</v>
+      <c r="A58" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B58" t="s">
         <v>231</v>
@@ -5696,14 +5700,14 @@
         <v>9000</v>
       </c>
       <c r="J58" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A59" t="s">
-        <v>582</v>
+      <c r="A59" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B59" t="s">
         <v>231</v>
@@ -5730,14 +5734,14 @@
         <v>20000</v>
       </c>
       <c r="J59" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A60" t="s">
-        <v>582</v>
+      <c r="A60" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B60" t="s">
         <v>241</v>
@@ -5764,14 +5768,14 @@
         <v>20000</v>
       </c>
       <c r="J60" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A61" t="s">
-        <v>582</v>
+      <c r="A61" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B61" t="s">
         <v>241</v>
@@ -5798,14 +5802,14 @@
         <v>25000</v>
       </c>
       <c r="J61" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A62" t="s">
-        <v>582</v>
+      <c r="A62" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B62" t="s">
         <v>246</v>
@@ -5832,14 +5836,14 @@
         <v>0</v>
       </c>
       <c r="J62" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" ht="13.75" customHeight="1">
-      <c r="A63" t="s">
-        <v>582</v>
+      <c r="A63" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B63" t="s">
         <v>246</v>
@@ -5866,7 +5870,7 @@
         <v>30000</v>
       </c>
       <c r="J63" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -5900,7 +5904,7 @@
         <v>15000</v>
       </c>
       <c r="J64" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
@@ -5934,7 +5938,7 @@
         <v>16000</v>
       </c>
       <c r="J65" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
@@ -5968,7 +5972,7 @@
         <v>16900</v>
       </c>
       <c r="J66" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
@@ -6002,7 +6006,7 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
@@ -6036,7 +6040,7 @@
         <v>20000</v>
       </c>
       <c r="J68" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
@@ -6070,7 +6074,7 @@
         <v>25000</v>
       </c>
       <c r="J69" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
@@ -6104,7 +6108,7 @@
         <v>20000</v>
       </c>
       <c r="J70" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
@@ -6138,7 +6142,7 @@
         <v>52000</v>
       </c>
       <c r="J71" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
@@ -6172,7 +6176,7 @@
         <v>52000</v>
       </c>
       <c r="J72" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
@@ -6206,7 +6210,7 @@
         <v>32727</v>
       </c>
       <c r="J73" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
@@ -6240,7 +6244,7 @@
         <v>22000</v>
       </c>
       <c r="J74" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
@@ -6274,7 +6278,7 @@
         <v>22000</v>
       </c>
       <c r="J75" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
@@ -6308,7 +6312,7 @@
         <v>22500</v>
       </c>
       <c r="J76" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
@@ -6342,7 +6346,7 @@
         <v>15000</v>
       </c>
       <c r="J77" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
@@ -6376,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="J78" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
@@ -6410,7 +6414,7 @@
         <v>20000</v>
       </c>
       <c r="J79" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
@@ -6444,7 +6448,7 @@
         <v>30000</v>
       </c>
       <c r="J80" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
@@ -6478,7 +6482,7 @@
         <v>30000</v>
       </c>
       <c r="J81" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
@@ -6512,7 +6516,7 @@
         <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
@@ -6546,7 +6550,7 @@
         <v>0</v>
       </c>
       <c r="J83" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
@@ -6580,7 +6584,7 @@
         <v>60900</v>
       </c>
       <c r="J84" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
@@ -6614,7 +6618,7 @@
         <v>12200</v>
       </c>
       <c r="J85" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
@@ -6648,7 +6652,7 @@
         <v>10000</v>
       </c>
       <c r="J86" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
@@ -6682,7 +6686,7 @@
         <v>80000</v>
       </c>
       <c r="J87" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
@@ -6692,7 +6696,7 @@
         <v>324</v>
       </c>
       <c r="B88" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C88" t="s">
         <v>338</v>
@@ -6716,7 +6720,7 @@
         <v>12000</v>
       </c>
       <c r="J88" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
@@ -6750,7 +6754,7 @@
         <v>25000</v>
       </c>
       <c r="J89" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
@@ -6784,7 +6788,7 @@
         <v>39000</v>
       </c>
       <c r="J90" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="K90" s="5"/>
       <c r="L90" s="5"/>
@@ -6797,7 +6801,7 @@
         <v>347</v>
       </c>
       <c r="C91" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D91" t="s">
         <v>348</v>
@@ -6818,7 +6822,7 @@
         <v>31500</v>
       </c>
       <c r="J91" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="K91" s="5"/>
       <c r="L91" s="5"/>
@@ -6828,7 +6832,7 @@
         <v>324</v>
       </c>
       <c r="B92" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C92" t="s">
         <v>350</v>
@@ -6852,7 +6856,7 @@
         <v>14200</v>
       </c>
       <c r="J92" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K92" s="5"/>
       <c r="L92" s="5"/>
@@ -6862,7 +6866,7 @@
         <v>324</v>
       </c>
       <c r="B93" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C93" t="s">
         <v>353</v>
@@ -6886,7 +6890,7 @@
         <v>10000</v>
       </c>
       <c r="J93" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="K93" s="5"/>
       <c r="L93" s="5"/>
@@ -6920,7 +6924,7 @@
         <v>10600</v>
       </c>
       <c r="J94" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
@@ -6954,7 +6958,7 @@
         <v>45000</v>
       </c>
       <c r="J95" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="K95" s="5"/>
       <c r="L95" s="5"/>
@@ -6964,7 +6968,7 @@
         <v>314</v>
       </c>
       <c r="B96" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C96" t="s">
         <v>362</v>
@@ -6988,7 +6992,7 @@
         <v>30000</v>
       </c>
       <c r="J96" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="K96" s="5"/>
       <c r="L96" s="5"/>
@@ -6998,10 +7002,10 @@
         <v>314</v>
       </c>
       <c r="B97" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C97" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D97" s="36" t="s">
         <v>38</v>
@@ -7013,7 +7017,7 @@
         <v>99</v>
       </c>
       <c r="G97" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H97" t="s">
         <v>40</v>
@@ -7028,13 +7032,13 @@
         <v>62</v>
       </c>
       <c r="B98" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C98" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D98" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E98" t="s">
         <v>53</v>
@@ -7043,7 +7047,7 @@
         <v>35</v>
       </c>
       <c r="G98" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="H98" t="s">
         <v>17</v>
@@ -7058,10 +7062,10 @@
         <v>314</v>
       </c>
       <c r="B99" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C99" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D99" t="s">
         <v>38</v>
@@ -7073,7 +7077,7 @@
         <v>528</v>
       </c>
       <c r="G99" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H99" t="s">
         <v>46</v>
@@ -7088,10 +7092,10 @@
         <v>62</v>
       </c>
       <c r="B100" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C100" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D100" t="s">
         <v>38</v>
@@ -7103,7 +7107,7 @@
         <v>99</v>
       </c>
       <c r="G100" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H100" t="s">
         <v>57</v>
@@ -7118,13 +7122,13 @@
         <v>62</v>
       </c>
       <c r="B101" t="s">
+        <v>632</v>
+      </c>
+      <c r="C101" t="s">
+        <v>633</v>
+      </c>
+      <c r="D101" t="s">
         <v>634</v>
-      </c>
-      <c r="C101" t="s">
-        <v>635</v>
-      </c>
-      <c r="D101" t="s">
-        <v>636</v>
       </c>
       <c r="E101" t="s">
         <v>14</v>
@@ -7133,7 +7137,7 @@
         <v>35</v>
       </c>
       <c r="G101" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H101" t="s">
         <v>236</v>
@@ -7148,10 +7152,10 @@
         <v>62</v>
       </c>
       <c r="B102" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C102" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D102" t="s">
         <v>38</v>
@@ -7163,7 +7167,7 @@
         <v>35</v>
       </c>
       <c r="G102" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H102" t="s">
         <v>40</v>
@@ -7178,10 +7182,10 @@
         <v>314</v>
       </c>
       <c r="B103" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C103" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D103" t="s">
         <v>38</v>
@@ -7193,7 +7197,7 @@
         <v>66</v>
       </c>
       <c r="G103" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="H103" t="s">
         <v>40</v>
@@ -7208,10 +7212,10 @@
         <v>314</v>
       </c>
       <c r="B104" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C104" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D104" t="s">
         <v>328</v>
@@ -7223,7 +7227,7 @@
         <v>66</v>
       </c>
       <c r="G104" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H104" t="s">
         <v>40</v>
@@ -7238,10 +7242,10 @@
         <v>314</v>
       </c>
       <c r="B105" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C105" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D105" t="s">
         <v>354</v>
@@ -7253,7 +7257,7 @@
         <v>257</v>
       </c>
       <c r="G105" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H105" t="s">
         <v>205</v>
@@ -7268,10 +7272,10 @@
         <v>62</v>
       </c>
       <c r="B106" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C106" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D106" t="s">
         <v>38</v>
@@ -7283,7 +7287,7 @@
         <v>66</v>
       </c>
       <c r="G106" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H106" t="s">
         <v>40</v>
@@ -7298,10 +7302,10 @@
         <v>62</v>
       </c>
       <c r="B107" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C107" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D107" t="s">
         <v>334</v>
@@ -7313,7 +7317,7 @@
         <v>35</v>
       </c>
       <c r="G107" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H107" t="s">
         <v>17</v>
@@ -7328,10 +7332,10 @@
         <v>62</v>
       </c>
       <c r="B108" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C108" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D108" t="s">
         <v>334</v>
@@ -7343,7 +7347,7 @@
         <v>257</v>
       </c>
       <c r="G108" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H108" t="s">
         <v>40</v>
@@ -7358,10 +7362,10 @@
         <v>314</v>
       </c>
       <c r="B109" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C109" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D109" t="s">
         <v>354</v>
@@ -7373,10 +7377,10 @@
         <v>99</v>
       </c>
       <c r="G109" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H109" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="I109"/>
       <c r="J109"/>
@@ -7388,10 +7392,10 @@
         <v>62</v>
       </c>
       <c r="B110" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C110" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D110" t="s">
         <v>334</v>
@@ -7403,7 +7407,7 @@
         <v>257</v>
       </c>
       <c r="G110" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H110" t="s">
         <v>215</v>
@@ -7418,10 +7422,10 @@
         <v>62</v>
       </c>
       <c r="B111" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C111" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D111" t="s">
         <v>334</v>
@@ -7433,7 +7437,7 @@
         <v>66</v>
       </c>
       <c r="G111" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H111" t="s">
         <v>17</v>
@@ -7448,10 +7452,10 @@
         <v>314</v>
       </c>
       <c r="B112" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C112" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D112" t="s">
         <v>88</v>
@@ -7463,7 +7467,7 @@
         <v>35</v>
       </c>
       <c r="G112" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="H112" t="s">
         <v>46</v>
@@ -7478,10 +7482,10 @@
         <v>314</v>
       </c>
       <c r="B113" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C113" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D113" t="s">
         <v>38</v>
@@ -7493,7 +7497,7 @@
         <v>355</v>
       </c>
       <c r="G113" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H113" t="s">
         <v>268</v>
@@ -7504,26 +7508,26 @@
       <c r="L113" s="5"/>
     </row>
     <row r="114" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A114" t="s">
-        <v>582</v>
+      <c r="A114" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B114" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C114" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D114" t="s">
         <v>184</v>
       </c>
       <c r="E114" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F114" t="s">
         <v>96</v>
       </c>
       <c r="G114" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H114" t="s">
         <v>236</v>
@@ -7538,10 +7542,10 @@
         <v>314</v>
       </c>
       <c r="B115" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C115" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D115" t="s">
         <v>38</v>
@@ -7553,7 +7557,7 @@
         <v>66</v>
       </c>
       <c r="G115" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H115" t="s">
         <v>276</v>
@@ -7568,10 +7572,10 @@
         <v>314</v>
       </c>
       <c r="B116" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C116" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D116" t="s">
         <v>334</v>
@@ -7583,7 +7587,7 @@
         <v>203</v>
       </c>
       <c r="G116" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="H116" t="s">
         <v>276</v>
@@ -7598,7 +7602,7 @@
         <v>62</v>
       </c>
       <c r="B117" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C117" t="s">
         <v>336</v>
@@ -7628,10 +7632,10 @@
         <v>62</v>
       </c>
       <c r="B118" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C118" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D118" t="s">
         <v>88</v>
@@ -7643,7 +7647,7 @@
         <v>355</v>
       </c>
       <c r="G118" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="H118" t="s">
         <v>46</v>
@@ -7654,11 +7658,11 @@
       <c r="L118" s="5"/>
     </row>
     <row r="119" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A119" t="s">
-        <v>582</v>
+      <c r="A119" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B119" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C119" s="36" t="s">
         <v>194</v>
@@ -7667,13 +7671,13 @@
         <v>38</v>
       </c>
       <c r="E119" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F119" t="s">
         <v>35</v>
       </c>
       <c r="G119" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="H119" t="s">
         <v>17</v>
@@ -7686,17 +7690,17 @@
       <c r="L119" s="5"/>
     </row>
     <row r="120" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A120" t="s">
-        <v>582</v>
+      <c r="A120" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B120" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C120" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D120" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E120" t="s">
         <v>14</v>
@@ -7705,7 +7709,7 @@
         <v>66</v>
       </c>
       <c r="G120" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H120" t="s">
         <v>17</v>
@@ -7716,17 +7720,17 @@
       <c r="L120" s="5"/>
     </row>
     <row r="121" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A121" t="s">
-        <v>582</v>
+      <c r="A121" s="37" t="s">
+        <v>728</v>
       </c>
       <c r="B121" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C121" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D121" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E121" t="s">
         <v>53</v>
@@ -7735,7 +7739,7 @@
         <v>257</v>
       </c>
       <c r="G121" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="H121" t="s">
         <v>236</v>
@@ -7747,25 +7751,25 @@
     </row>
     <row r="122" spans="1:12" ht="14.5" customHeight="1">
       <c r="A122" t="s">
+        <v>688</v>
+      </c>
+      <c r="B122" t="s">
+        <v>689</v>
+      </c>
+      <c r="C122" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B122" t="s">
-        <v>691</v>
-      </c>
-      <c r="C122" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D122" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E122" t="s">
         <v>75</v>
       </c>
       <c r="F122" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G122" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H122" t="s">
         <v>17</v>
@@ -7777,16 +7781,16 @@
     </row>
     <row r="123" spans="1:12" ht="14.5" customHeight="1">
       <c r="A123" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B123" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C123" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D123" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E123" t="s">
         <v>53</v>
@@ -7795,7 +7799,7 @@
         <v>99</v>
       </c>
       <c r="G123" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H123" t="s">
         <v>57</v>
@@ -7807,25 +7811,25 @@
     </row>
     <row r="124" spans="1:12" ht="14.5" customHeight="1">
       <c r="A124" t="s">
+        <v>688</v>
+      </c>
+      <c r="B124" t="s">
+        <v>696</v>
+      </c>
+      <c r="C124" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B124" t="s">
-        <v>698</v>
-      </c>
-      <c r="C124" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D124" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E124" t="s">
         <v>75</v>
       </c>
       <c r="F124" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G124" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H124" t="s">
         <v>17</v>
@@ -7837,16 +7841,16 @@
     </row>
     <row r="125" spans="1:12" ht="14.5" customHeight="1">
       <c r="A125" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B125" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C125" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D125" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E125" t="s">
         <v>53</v>
@@ -7855,7 +7859,7 @@
         <v>99</v>
       </c>
       <c r="G125" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H125" t="s">
         <v>57</v>
@@ -7867,25 +7871,25 @@
     </row>
     <row r="126" spans="1:12" ht="14.5" customHeight="1">
       <c r="A126" t="s">
+        <v>688</v>
+      </c>
+      <c r="B126" t="s">
+        <v>697</v>
+      </c>
+      <c r="C126" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B126" t="s">
-        <v>699</v>
-      </c>
-      <c r="C126" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D126" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E126" t="s">
         <v>75</v>
       </c>
       <c r="F126" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G126" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H126" t="s">
         <v>17</v>
@@ -7897,16 +7901,16 @@
     </row>
     <row r="127" spans="1:12" ht="14.5" customHeight="1">
       <c r="A127" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B127" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C127" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D127" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E127" t="s">
         <v>53</v>
@@ -7915,7 +7919,7 @@
         <v>99</v>
       </c>
       <c r="G127" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H127" t="s">
         <v>57</v>
@@ -7927,25 +7931,25 @@
     </row>
     <row r="128" spans="1:12" ht="14.5" customHeight="1">
       <c r="A128" t="s">
+        <v>688</v>
+      </c>
+      <c r="B128" t="s">
+        <v>698</v>
+      </c>
+      <c r="C128" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B128" t="s">
-        <v>700</v>
-      </c>
-      <c r="C128" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D128" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E128" t="s">
         <v>75</v>
       </c>
       <c r="F128" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G128" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H128" t="s">
         <v>17</v>
@@ -7957,16 +7961,16 @@
     </row>
     <row r="129" spans="1:12" ht="14.5" customHeight="1">
       <c r="A129" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B129" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C129" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D129" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E129" t="s">
         <v>53</v>
@@ -7975,7 +7979,7 @@
         <v>99</v>
       </c>
       <c r="G129" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H129" t="s">
         <v>57</v>
@@ -7987,46 +7991,48 @@
     </row>
     <row r="130" spans="1:12" ht="14.5" customHeight="1">
       <c r="A130" t="s">
+        <v>688</v>
+      </c>
+      <c r="B130" t="s">
+        <v>699</v>
+      </c>
+      <c r="C130" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B130" t="s">
-        <v>701</v>
-      </c>
-      <c r="C130" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D130" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E130" t="s">
         <v>75</v>
       </c>
       <c r="F130" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G130" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H130" t="s">
         <v>17</v>
       </c>
       <c r="I130"/>
-      <c r="J130"/>
+      <c r="J130" t="s">
+        <v>727</v>
+      </c>
       <c r="K130" s="5"/>
       <c r="L130" s="5"/>
     </row>
     <row r="131" spans="1:12" ht="14.5" customHeight="1">
       <c r="A131" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B131" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C131" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D131" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E131" t="s">
         <v>53</v>
@@ -8035,7 +8041,7 @@
         <v>99</v>
       </c>
       <c r="G131" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H131" t="s">
         <v>57</v>
@@ -8047,25 +8053,25 @@
     </row>
     <row r="132" spans="1:12" ht="14.5" customHeight="1">
       <c r="A132" t="s">
+        <v>688</v>
+      </c>
+      <c r="B132" t="s">
+        <v>700</v>
+      </c>
+      <c r="C132" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B132" t="s">
-        <v>702</v>
-      </c>
-      <c r="C132" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D132" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E132" t="s">
         <v>75</v>
       </c>
       <c r="F132" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G132" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H132" t="s">
         <v>17</v>
@@ -8077,16 +8083,16 @@
     </row>
     <row r="133" spans="1:12" ht="14.5" customHeight="1">
       <c r="A133" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B133" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C133" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D133" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E133" t="s">
         <v>53</v>
@@ -8095,7 +8101,7 @@
         <v>99</v>
       </c>
       <c r="G133" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H133" t="s">
         <v>57</v>
@@ -8107,25 +8113,25 @@
     </row>
     <row r="134" spans="1:12" ht="14.5" customHeight="1">
       <c r="A134" t="s">
+        <v>688</v>
+      </c>
+      <c r="B134" t="s">
+        <v>701</v>
+      </c>
+      <c r="C134" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B134" t="s">
-        <v>703</v>
-      </c>
-      <c r="C134" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D134" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E134" t="s">
         <v>75</v>
       </c>
       <c r="F134" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G134" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H134" t="s">
         <v>17</v>
@@ -8137,16 +8143,16 @@
     </row>
     <row r="135" spans="1:12" ht="14.5" customHeight="1">
       <c r="A135" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B135" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C135" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D135" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E135" t="s">
         <v>53</v>
@@ -8155,7 +8161,7 @@
         <v>99</v>
       </c>
       <c r="G135" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H135" t="s">
         <v>57</v>
@@ -8167,25 +8173,25 @@
     </row>
     <row r="136" spans="1:12" ht="14.5" customHeight="1">
       <c r="A136" t="s">
+        <v>688</v>
+      </c>
+      <c r="B136" t="s">
+        <v>702</v>
+      </c>
+      <c r="C136" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B136" t="s">
-        <v>704</v>
-      </c>
-      <c r="C136" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D136" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E136" t="s">
         <v>75</v>
       </c>
       <c r="F136" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G136" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H136" t="s">
         <v>17</v>
@@ -8197,16 +8203,16 @@
     </row>
     <row r="137" spans="1:12" ht="14.5" customHeight="1">
       <c r="A137" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B137" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C137" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D137" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E137" t="s">
         <v>53</v>
@@ -8215,7 +8221,7 @@
         <v>99</v>
       </c>
       <c r="G137" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H137" t="s">
         <v>57</v>
@@ -8227,25 +8233,25 @@
     </row>
     <row r="138" spans="1:12" ht="14.5" customHeight="1">
       <c r="A138" t="s">
+        <v>688</v>
+      </c>
+      <c r="B138" t="s">
+        <v>703</v>
+      </c>
+      <c r="C138" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B138" t="s">
-        <v>705</v>
-      </c>
-      <c r="C138" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D138" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E138" t="s">
         <v>75</v>
       </c>
       <c r="F138" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G138" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H138" t="s">
         <v>17</v>
@@ -8257,16 +8263,16 @@
     </row>
     <row r="139" spans="1:12" ht="14.5" customHeight="1">
       <c r="A139" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B139" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C139" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D139" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E139" t="s">
         <v>53</v>
@@ -8275,7 +8281,7 @@
         <v>99</v>
       </c>
       <c r="G139" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H139" t="s">
         <v>57</v>
@@ -8287,16 +8293,16 @@
     </row>
     <row r="140" spans="1:12" ht="14.5" customHeight="1">
       <c r="A140" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B140" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C140" s="36" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D140" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E140" t="s">
         <v>23</v>
@@ -8305,7 +8311,7 @@
         <v>257</v>
       </c>
       <c r="G140" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="H140" t="s">
         <v>268</v>
@@ -8317,16 +8323,16 @@
     </row>
     <row r="141" spans="1:12" ht="14.5" customHeight="1">
       <c r="A141" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B141" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C141" s="36" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D141" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E141" t="s">
         <v>14</v>
@@ -8335,7 +8341,7 @@
         <v>35</v>
       </c>
       <c r="G141" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="H141" t="s">
         <v>40</v>
@@ -8347,25 +8353,25 @@
     </row>
     <row r="142" spans="1:12" ht="14.5" customHeight="1">
       <c r="A142" t="s">
+        <v>688</v>
+      </c>
+      <c r="B142" t="s">
+        <v>709</v>
+      </c>
+      <c r="C142" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B142" t="s">
-        <v>711</v>
-      </c>
-      <c r="C142" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D142" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E142" t="s">
         <v>75</v>
       </c>
       <c r="F142" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G142" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H142" t="s">
         <v>17</v>
@@ -8377,16 +8383,16 @@
     </row>
     <row r="143" spans="1:12" ht="14.5" customHeight="1">
       <c r="A143" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B143" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C143" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D143" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E143" t="s">
         <v>53</v>
@@ -8395,7 +8401,7 @@
         <v>99</v>
       </c>
       <c r="G143" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H143" t="s">
         <v>57</v>
@@ -8407,25 +8413,25 @@
     </row>
     <row r="144" spans="1:12" ht="14.5" customHeight="1">
       <c r="A144" t="s">
+        <v>688</v>
+      </c>
+      <c r="B144" t="s">
+        <v>710</v>
+      </c>
+      <c r="C144" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="B144" t="s">
-        <v>712</v>
-      </c>
-      <c r="C144" s="36" t="s">
-        <v>692</v>
-      </c>
       <c r="D144" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E144" t="s">
         <v>75</v>
       </c>
       <c r="F144" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G144" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H144" t="s">
         <v>17</v>
@@ -8437,16 +8443,16 @@
     </row>
     <row r="145" spans="1:12" ht="14.5" customHeight="1">
       <c r="A145" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B145" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C145" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D145" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E145" t="s">
         <v>53</v>
@@ -8455,7 +8461,7 @@
         <v>99</v>
       </c>
       <c r="G145" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H145" t="s">
         <v>57</v>
@@ -8466,17 +8472,17 @@
       <c r="L145" s="5"/>
     </row>
     <row r="146" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A146" t="s">
-        <v>566</v>
+      <c r="A146" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B146" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C146" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D146" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E146" t="s">
         <v>23</v>
@@ -8485,7 +8491,7 @@
         <v>96</v>
       </c>
       <c r="G146" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="H146" t="s">
         <v>46</v>
@@ -8496,26 +8502,26 @@
       <c r="L146" s="5"/>
     </row>
     <row r="147" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A147" t="s">
-        <v>566</v>
+      <c r="A147" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B147" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C147" t="s">
+        <v>714</v>
+      </c>
+      <c r="D147" t="s">
+        <v>715</v>
+      </c>
+      <c r="E147" t="s">
         <v>716</v>
-      </c>
-      <c r="D147" t="s">
-        <v>717</v>
-      </c>
-      <c r="E147" t="s">
-        <v>718</v>
       </c>
       <c r="F147" t="s">
         <v>35</v>
       </c>
       <c r="G147" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="H147" t="s">
         <v>236</v>
@@ -8526,17 +8532,17 @@
       <c r="L147" s="5"/>
     </row>
     <row r="148" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A148" t="s">
-        <v>566</v>
+      <c r="A148" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B148" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C148" s="36" t="s">
         <v>344</v>
       </c>
       <c r="D148" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E148" t="s">
         <v>27</v>
@@ -8556,17 +8562,17 @@
       <c r="L148" s="5"/>
     </row>
     <row r="149" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A149" t="s">
-        <v>566</v>
+      <c r="A149" s="37" t="s">
+        <v>729</v>
       </c>
       <c r="B149" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C149" s="36" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D149" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E149" t="s">
         <v>27</v>
@@ -8575,7 +8581,7 @@
         <v>35</v>
       </c>
       <c r="G149" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="H149" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
fix product details dan merged manually fitur reviews yang udah shasi benerin
</commit_message>
<xml_diff>
--- a/static/data/dataset.xlsx
+++ b/static/data/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valizanadya/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A4D6D77-FCA8-6641-A8C0-71B2D7F1F092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C351D036-9F6D-5642-BF3A-E5D7B43D216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4005,8 +4005,8 @@
   </sheetPr>
   <dimension ref="A1:L214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C105" workbookViewId="0">
+      <selection activeCell="I152" sqref="I152:I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4458,7 +4458,9 @@
       <c r="H13" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="36"/>
+      <c r="I13" s="36">
+        <v>0</v>
+      </c>
       <c r="J13" s="37" t="s">
         <v>505</v>
       </c>
@@ -4490,7 +4492,9 @@
       <c r="H14" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I14" s="36"/>
+      <c r="I14" s="36">
+        <v>0</v>
+      </c>
       <c r="J14" s="37" t="s">
         <v>505</v>
       </c>
@@ -4590,7 +4594,9 @@
       <c r="H17" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="I17" s="36"/>
+      <c r="I17" s="36">
+        <v>0</v>
+      </c>
       <c r="J17" s="37" t="s">
         <v>512</v>
       </c>
@@ -4622,7 +4628,9 @@
       <c r="H18" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="36"/>
+      <c r="I18" s="36">
+        <v>0</v>
+      </c>
       <c r="J18" s="37" t="s">
         <v>514</v>
       </c>
@@ -4654,7 +4662,9 @@
       <c r="H19" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I19" s="36"/>
+      <c r="I19" s="36">
+        <v>0</v>
+      </c>
       <c r="J19" s="37" t="s">
         <v>516</v>
       </c>
@@ -4686,7 +4696,9 @@
       <c r="H20" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="36"/>
+      <c r="I20" s="36">
+        <v>0</v>
+      </c>
       <c r="J20" s="37" t="s">
         <v>516</v>
       </c>
@@ -4888,7 +4900,9 @@
       <c r="H26" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="36"/>
+      <c r="I26" s="36">
+        <v>0</v>
+      </c>
       <c r="J26" s="37" t="s">
         <v>527</v>
       </c>
@@ -4920,7 +4934,9 @@
       <c r="H27" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I27" s="36"/>
+      <c r="I27" s="36">
+        <v>0</v>
+      </c>
       <c r="J27" s="37" t="s">
         <v>529</v>
       </c>
@@ -4986,7 +5002,9 @@
       <c r="H29" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="36"/>
+      <c r="I29" s="36">
+        <v>0</v>
+      </c>
       <c r="J29" s="37" t="s">
         <v>532</v>
       </c>
@@ -5018,7 +5036,9 @@
       <c r="H30" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I30" s="36"/>
+      <c r="I30" s="36">
+        <v>0</v>
+      </c>
       <c r="J30" s="37" t="s">
         <v>532</v>
       </c>
@@ -5048,7 +5068,9 @@
       <c r="H31" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="36"/>
+      <c r="I31" s="36">
+        <v>0</v>
+      </c>
       <c r="J31" s="37" t="s">
         <v>534</v>
       </c>
@@ -5080,7 +5102,9 @@
       <c r="H32" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="36"/>
+      <c r="I32" s="36">
+        <v>0</v>
+      </c>
       <c r="J32" s="37" t="s">
         <v>535</v>
       </c>
@@ -5112,7 +5136,9 @@
       <c r="H33" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="I33" s="36"/>
+      <c r="I33" s="36">
+        <v>0</v>
+      </c>
       <c r="J33" s="37" t="s">
         <v>535</v>
       </c>
@@ -5144,7 +5170,9 @@
       <c r="H34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="36"/>
+      <c r="I34" s="36">
+        <v>0</v>
+      </c>
       <c r="J34" s="37" t="s">
         <v>536</v>
       </c>
@@ -5276,7 +5304,9 @@
       <c r="H38" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I38" s="36"/>
+      <c r="I38" s="36">
+        <v>0</v>
+      </c>
       <c r="J38" s="37" t="s">
         <v>539</v>
       </c>
@@ -5308,7 +5338,9 @@
       <c r="H39" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="36"/>
+      <c r="I39" s="36">
+        <v>0</v>
+      </c>
       <c r="J39" s="37" t="s">
         <v>540</v>
       </c>
@@ -5340,7 +5372,9 @@
       <c r="H40" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I40" s="36"/>
+      <c r="I40" s="36">
+        <v>0</v>
+      </c>
       <c r="J40" s="37" t="s">
         <v>540</v>
       </c>
@@ -5508,7 +5542,9 @@
       <c r="H45" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I45" s="36"/>
+      <c r="I45" s="36">
+        <v>0</v>
+      </c>
       <c r="J45" s="37" t="s">
         <v>550</v>
       </c>
@@ -5540,7 +5576,9 @@
       <c r="H46" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I46" s="36"/>
+      <c r="I46" s="36">
+        <v>0</v>
+      </c>
       <c r="J46" s="37" t="s">
         <v>550</v>
       </c>
@@ -5572,7 +5610,9 @@
       <c r="H47" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="I47" s="36"/>
+      <c r="I47" s="36">
+        <v>0</v>
+      </c>
       <c r="J47" s="37" t="s">
         <v>550</v>
       </c>
@@ -5604,7 +5644,9 @@
       <c r="H48" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="I48" s="36"/>
+      <c r="I48" s="36">
+        <v>0</v>
+      </c>
       <c r="J48" s="37" t="s">
         <v>552</v>
       </c>
@@ -5636,7 +5678,9 @@
       <c r="H49" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I49" s="36"/>
+      <c r="I49" s="36">
+        <v>0</v>
+      </c>
       <c r="J49" s="37" t="s">
         <v>552</v>
       </c>
@@ -5668,7 +5712,9 @@
       <c r="H50" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="I50" s="36"/>
+      <c r="I50" s="36">
+        <v>0</v>
+      </c>
       <c r="J50" s="37" t="s">
         <v>553</v>
       </c>
@@ -5700,7 +5746,9 @@
       <c r="H51" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="I51" s="36"/>
+      <c r="I51" s="36">
+        <v>0</v>
+      </c>
       <c r="J51" s="37" t="s">
         <v>553</v>
       </c>
@@ -5730,7 +5778,9 @@
       <c r="H52" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I52" s="36"/>
+      <c r="I52" s="36">
+        <v>0</v>
+      </c>
       <c r="J52" s="37" t="s">
         <v>555</v>
       </c>
@@ -5828,7 +5878,9 @@
       <c r="H55" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I55" s="36"/>
+      <c r="I55" s="36">
+        <v>0</v>
+      </c>
       <c r="J55" s="37" t="s">
         <v>560</v>
       </c>
@@ -5860,7 +5912,9 @@
       <c r="H56" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="I56" s="36"/>
+      <c r="I56" s="36">
+        <v>0</v>
+      </c>
       <c r="J56" s="37" t="s">
         <v>561</v>
       </c>
@@ -6062,7 +6116,9 @@
       <c r="H62" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I62" s="36"/>
+      <c r="I62" s="36">
+        <v>0</v>
+      </c>
       <c r="J62" s="37" t="s">
         <v>567</v>
       </c>
@@ -6230,7 +6286,9 @@
       <c r="H67" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I67" s="36"/>
+      <c r="I67" s="36">
+        <v>0</v>
+      </c>
       <c r="J67" s="37" t="s">
         <v>572</v>
       </c>
@@ -6602,7 +6660,9 @@
       <c r="H78" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I78" s="36"/>
+      <c r="I78" s="36">
+        <v>0</v>
+      </c>
       <c r="J78" s="37" t="s">
         <v>581</v>
       </c>
@@ -6736,7 +6796,9 @@
       <c r="H82" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="I82" s="36"/>
+      <c r="I82" s="36">
+        <v>0</v>
+      </c>
       <c r="J82" s="37" t="s">
         <v>585</v>
       </c>
@@ -6768,7 +6830,9 @@
       <c r="H83" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="I83" s="36"/>
+      <c r="I83" s="36">
+        <v>0</v>
+      </c>
       <c r="J83" s="37" t="s">
         <v>708</v>
       </c>
@@ -7242,7 +7306,9 @@
       <c r="H97" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I97" s="36"/>
+      <c r="I97" s="36">
+        <v>0</v>
+      </c>
       <c r="J97" s="37" t="s">
         <v>717</v>
       </c>
@@ -7274,7 +7340,9 @@
       <c r="H98" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I98" s="36"/>
+      <c r="I98" s="36">
+        <v>0</v>
+      </c>
       <c r="J98" s="37" t="s">
         <v>718</v>
       </c>
@@ -7306,7 +7374,9 @@
       <c r="H99" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I99" s="36"/>
+      <c r="I99" s="36">
+        <v>0</v>
+      </c>
       <c r="J99" s="37" t="s">
         <v>719</v>
       </c>
@@ -7338,7 +7408,9 @@
       <c r="H100" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="I100" s="36"/>
+      <c r="I100" s="36">
+        <v>0</v>
+      </c>
       <c r="J100" s="37" t="s">
         <v>720</v>
       </c>
@@ -7370,7 +7442,9 @@
       <c r="H101" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I101" s="36"/>
+      <c r="I101" s="36">
+        <v>0</v>
+      </c>
       <c r="J101" s="37" t="s">
         <v>721</v>
       </c>
@@ -7436,7 +7510,9 @@
       <c r="H103" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I103" s="36"/>
+      <c r="I103" s="36">
+        <v>0</v>
+      </c>
       <c r="J103" s="37" t="s">
         <v>725</v>
       </c>
@@ -7468,7 +7544,9 @@
       <c r="H104" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I104" s="36"/>
+      <c r="I104" s="36">
+        <v>0</v>
+      </c>
       <c r="J104" s="37" t="s">
         <v>726</v>
       </c>
@@ -7534,7 +7612,9 @@
       <c r="H106" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I106" s="36"/>
+      <c r="I106" s="36">
+        <v>0</v>
+      </c>
       <c r="J106" s="37" t="s">
         <v>728</v>
       </c>
@@ -7634,7 +7714,9 @@
       <c r="H109" s="36" t="s">
         <v>632</v>
       </c>
-      <c r="I109" s="36"/>
+      <c r="I109" s="36">
+        <v>0</v>
+      </c>
       <c r="J109" s="37" t="s">
         <v>731</v>
       </c>
@@ -7768,7 +7850,9 @@
       <c r="H113" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I113" s="36"/>
+      <c r="I113" s="36">
+        <v>0</v>
+      </c>
       <c r="J113" s="37" t="s">
         <v>737</v>
       </c>
@@ -7800,7 +7884,9 @@
       <c r="H114" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I114" s="36"/>
+      <c r="I114" s="36">
+        <v>0</v>
+      </c>
       <c r="J114" s="37" t="s">
         <v>741</v>
       </c>
@@ -7866,7 +7952,9 @@
       <c r="H116" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="I116" s="36"/>
+      <c r="I116" s="36">
+        <v>0</v>
+      </c>
       <c r="J116" s="37" t="s">
         <v>745</v>
       </c>
@@ -7898,7 +7986,9 @@
       <c r="H117" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I117" s="36"/>
+      <c r="I117" s="36">
+        <v>0</v>
+      </c>
       <c r="J117" s="37" t="s">
         <v>746</v>
       </c>
@@ -8576,7 +8666,9 @@
       <c r="H137" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I137" s="36"/>
+      <c r="I137" s="36">
+        <v>0</v>
+      </c>
       <c r="J137" s="37" t="s">
         <v>771</v>
       </c>
@@ -8674,7 +8766,9 @@
       <c r="H140" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="I140" s="36"/>
+      <c r="I140" s="36">
+        <v>0</v>
+      </c>
       <c r="J140" s="37" t="s">
         <v>775</v>
       </c>
@@ -8910,7 +9004,9 @@
       <c r="H147" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I147" s="36"/>
+      <c r="I147" s="36">
+        <v>0</v>
+      </c>
       <c r="J147" s="37" t="s">
         <v>806</v>
       </c>
@@ -9078,7 +9174,9 @@
       <c r="H152" s="36" t="s">
         <v>829</v>
       </c>
-      <c r="I152" s="36"/>
+      <c r="I152" s="36">
+        <v>0</v>
+      </c>
       <c r="J152" s="37" t="s">
         <v>830</v>
       </c>
@@ -9108,7 +9206,9 @@
       <c r="H153" s="36" t="s">
         <v>829</v>
       </c>
-      <c r="I153" s="36"/>
+      <c r="I153" s="36">
+        <v>0</v>
+      </c>
       <c r="J153" s="37" t="s">
         <v>832</v>
       </c>
@@ -9140,7 +9240,9 @@
       <c r="H154" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I154" s="36"/>
+      <c r="I154" s="36">
+        <v>0</v>
+      </c>
       <c r="J154" s="37" t="s">
         <v>837</v>
       </c>
@@ -9172,7 +9274,9 @@
       <c r="H155" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I155" s="36"/>
+      <c r="I155" s="36">
+        <v>0</v>
+      </c>
       <c r="J155" s="37" t="s">
         <v>837</v>
       </c>

</xml_diff>